<commit_message>
upate regions censoring with AFE and AFW
</commit_message>
<xml_diff>
--- a/censoring.xlsx
+++ b/censoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\PIP-Data_QA\_aux\censoring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/acastanedaa_worldbank_org/Documents/WorldBank/DECDG/PIP/aux_data/aux_censoring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85573E1-B547-4674-B9AA-70BDAA34D6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{D85573E1-B547-4674-B9AA-70BDAA34D6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B162E7C1-9F2A-4F80-AF3A-EEFE13ECBAE8}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{83058514-9FE6-4DC6-9E73-CD4162A9D61C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{83058514-9FE6-4DC6-9E73-CD4162A9D61C}"/>
   </bookViews>
   <sheets>
     <sheet name="countries" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="33">
   <si>
     <t>country_code</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>PICES</t>
+  </si>
+  <si>
+    <t>AFE</t>
+  </si>
+  <si>
+    <t>AFW</t>
   </si>
 </sst>
 </file>
@@ -169,8 +175,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,19 +494,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F53354CC-896A-44EB-8E15-F8FFFE22A8E9}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.23046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.4609375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.4609375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +526,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -539,7 +546,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -559,7 +566,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -579,7 +586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -599,7 +606,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -619,7 +626,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -639,7 +646,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -659,7 +666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -679,7 +686,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -699,7 +706,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -719,7 +726,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -739,7 +746,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -759,7 +766,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -779,7 +786,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -799,7 +806,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -819,7 +826,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -839,7 +846,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -859,7 +866,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -879,7 +886,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -899,7 +906,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -919,7 +926,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -939,7 +946,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -959,7 +966,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -979,7 +986,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -999,7 +1006,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1019,7 +1026,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1039,7 +1046,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1059,7 +1066,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1079,7 +1086,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1099,7 +1106,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1119,7 +1126,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1139,7 +1146,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -1159,7 +1166,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -1179,7 +1186,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -1199,7 +1206,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>29</v>
       </c>
@@ -1219,7 +1226,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -1239,7 +1246,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>29</v>
       </c>
@@ -1268,19 +1275,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87DA734-60B7-4B5A-BCDA-01EB837E1664}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.07421875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1289,6 +1297,204 @@
       </c>
       <c r="C1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1981</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1982</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1983</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1984</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1985</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1986</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1987</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1988</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1989</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1990</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1991</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1992</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1997</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1981</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1982</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2007</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add eca and ohi 2021
</commit_message>
<xml_diff>
--- a/censoring.xlsx
+++ b/censoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/acastanedaa_worldbank_org/Documents/WorldBank/DECDG/PIP/aux_data/aux_censoring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{D85573E1-B547-4674-B9AA-70BDAA34D6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B162E7C1-9F2A-4F80-AF3A-EEFE13ECBAE8}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{D85573E1-B547-4674-B9AA-70BDAA34D6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{487DF20D-BBAF-4B44-B8DD-8254B83ED587}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{83058514-9FE6-4DC6-9E73-CD4162A9D61C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="35">
   <si>
     <t>country_code</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>AFW</t>
+  </si>
+  <si>
+    <t>ECA</t>
+  </si>
+  <si>
+    <t>OHI</t>
   </si>
 </sst>
 </file>
@@ -1275,10 +1281,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87DA734-60B7-4B5A-BCDA-01EB837E1664}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,6 +1503,28 @@
         <v>7</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2021</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2021</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>